<commit_message>
revert back to baseline - best results so far
</commit_message>
<xml_diff>
--- a/data/results/performance/performance_multigrid.xlsx
+++ b/data/results/performance/performance_multigrid.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!\2018\battery\battery\data\results\performance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!\battery\battery\data\results\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB094315-1FAA-44B9-92F0-26CE8ED762E3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73BE3DD-FB1C-458E-855D-FD337563BAE5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11580" activeTab="2" xr2:uid="{CCF8D299-8A86-4FA5-9802-73296FAB53F1}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="100">
   <si>
     <t>x</t>
   </si>
@@ -348,6 +348,9 @@
   <si>
     <t>9,15 vs 6,6</t>
   </si>
+  <si>
+    <t>v cycle, 2 levels, direct solver on second, 1e-6, xneg, zero first guess, unweighted interp &amp; restr, nonharmonic, direct coarsening</t>
+  </si>
 </sst>
 </file>
 
@@ -356,7 +359,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,16 +375,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -389,18 +416,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3624,10 +3675,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17AE62E-03D1-4E2F-9FFE-189D5E2D6059}">
-  <dimension ref="A2:N69"/>
+  <dimension ref="A2:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3636,7 +3687,7 @@
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -3650,7 +3701,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -3664,7 +3715,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -3672,7 +3723,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -3685,8 +3736,16 @@
       <c r="E5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q5" s="5"/>
+      <c r="R5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -3702,8 +3761,14 @@
       <c r="E6">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q6" s="5"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -3722,8 +3787,14 @@
       <c r="F7">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q7" s="5"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -3742,8 +3813,14 @@
       <c r="F8">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q8" s="5"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -3759,8 +3836,16 @@
       <c r="E9">
         <v>0.61</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -3782,16 +3867,56 @@
       <c r="G10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R11" s="5">
+        <v>8</v>
+      </c>
+      <c r="S11" s="5">
+        <v>5</v>
+      </c>
+      <c r="T11" s="5">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5">
+        <v>16</v>
+      </c>
+      <c r="S12" s="5">
+        <v>5</v>
+      </c>
+      <c r="T12" s="5">
+        <v>5.5E-2</v>
+      </c>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -3810,60 +3935,113 @@
       <c r="G13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5">
+        <v>32</v>
+      </c>
+      <c r="S13" s="5">
+        <v>6</v>
+      </c>
+      <c r="T13" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>5</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5">
+        <v>64</v>
+      </c>
+      <c r="S14" s="5">
+        <v>6</v>
+      </c>
+      <c r="T14" s="5">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4">
         <v>16</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>5</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="Q15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R15" s="5">
+        <v>8</v>
+      </c>
+      <c r="S15" s="5">
+        <v>11</v>
+      </c>
+      <c r="T15" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4">
         <v>32</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>6</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="E16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5">
+        <v>16</v>
+      </c>
+      <c r="S16" s="5">
+        <v>15</v>
+      </c>
+      <c r="T16" s="5">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4">
         <v>64</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>6</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="E17">
@@ -3872,18 +4050,30 @@
       <c r="F17" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5">
+        <v>32</v>
+      </c>
+      <c r="S17" s="5">
+        <v>15</v>
+      </c>
+      <c r="T17" s="5">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>8</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>11</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>0.33800000000000002</v>
       </c>
       <c r="E18">
@@ -3898,15 +4088,28 @@
       <c r="H18">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5">
+        <v>64</v>
+      </c>
+      <c r="S18" s="5">
+        <v>36</v>
+      </c>
+      <c r="T18" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4">
         <v>16</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>15</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>0.46</v>
       </c>
       <c r="E19">
@@ -3922,14 +4125,15 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4">
         <v>32</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>15</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>0.46</v>
       </c>
       <c r="E20">
@@ -3945,14 +4149,15 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4">
         <v>64</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>36</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>0.75</v>
       </c>
       <c r="E21">
@@ -3968,7 +4173,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -3982,7 +4187,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -3996,7 +4201,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -4007,7 +4212,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -4021,7 +4226,7 @@
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>16</v>
       </c>
@@ -4032,7 +4237,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>32</v>
       </c>
@@ -4043,7 +4248,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>64</v>
       </c>
@@ -4054,7 +4259,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>96</v>
       </c>
@@ -4065,7 +4270,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -4079,7 +4284,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>16</v>
       </c>
@@ -4568,6 +4773,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="R5:V9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Weighted interpolation using weights from different level
</commit_message>
<xml_diff>
--- a/data/results/performance/performance_multigrid.xlsx
+++ b/data/results/performance/performance_multigrid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!\2018\battery\battery\data\results\performance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!\battery\battery\data\results\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF33105C-99CC-4CBF-959E-D761D7E17BEF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB83249A-1A8D-4024-BF5C-DEC13BA50518}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11580" activeTab="3" xr2:uid="{CCF8D299-8A86-4FA5-9802-73296FAB53F1}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Boundary" sheetId="3" r:id="rId3"/>
     <sheet name="New Test" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="206">
   <si>
     <t>x</t>
   </si>
@@ -660,6 +660,15 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>empty, I = R'*8</t>
+  </si>
+  <si>
+    <t>I,R, trilinear weighted</t>
+  </si>
+  <si>
+    <t>Divergent</t>
   </si>
 </sst>
 </file>
@@ -4961,10 +4970,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EF2285-8896-4B10-84E1-CD5F722E2922}">
-  <dimension ref="A1:O185"/>
+  <dimension ref="A1:O192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L175" sqref="L175"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E192" sqref="E192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6995,6 +7004,56 @@
         <v>7.4499999999999997E-2</v>
       </c>
     </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>203</v>
+      </c>
+      <c r="E189" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>16</v>
+      </c>
+      <c r="B190">
+        <v>5</v>
+      </c>
+      <c r="C190">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="E190">
+        <v>5</v>
+      </c>
+      <c r="F190">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>16</v>
+      </c>
+      <c r="B192">
+        <v>64</v>
+      </c>
+      <c r="C192">
+        <v>0.82</v>
+      </c>
+      <c r="E192" t="s">
+        <v>202</v>
+      </c>
+      <c r="F192" t="s">
+        <v>202</v>
+      </c>
+      <c r="G192" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:F5"/>

</xml_diff>